<commit_message>
ci siamo dimenticati ieri
</commit_message>
<xml_diff>
--- a/aziende.xlsx
+++ b/aziende.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="327" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="255" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ditta" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
     <t>settore</t>
   </si>
   <si>
-    <t>sedeLegale</t>
+    <t>sedelegale</t>
   </si>
   <si>
     <t>citta</t>
@@ -268,16 +268,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,10 +282,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,256 +305,256 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="28.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.4241071428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.4241071428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.4285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="22.5669642857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.0803571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="2" width="13.4241071428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="28.8616071428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="26.5669642857143"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="2" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="30.5669642857143"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="2" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="2" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4241071428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.4241071428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5669642857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0803571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="13.4241071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.8616071428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5669642857143"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.5669642857143"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="J6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="0" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="0" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="0" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="0" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>